<commit_message>
Adds European biomass-based hydrogen
</commit_message>
<xml_diff>
--- a/rmnd_lca/data/additional_inventories/lci-hydrogen-wood-gasification.xlsx
+++ b/rmnd_lca/data/additional_inventories/lci-hydrogen-wood-gasification.xlsx
@@ -1,25 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0615525D-130B-4995-9446-8DD7270E1F38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1250" uniqueCount="91">
   <si>
     <t>Activity</t>
   </si>
@@ -283,12 +293,21 @@
   </si>
   <si>
     <t>Hydrogen, gaseous, 700 bar, from gasification of woody biomass in oxy-fired entrained flow gasifier, at H2 fuelling station</t>
+  </si>
+  <si>
+    <t>Europe without Switzerland</t>
+  </si>
+  <si>
+    <t>Hydrogen, gaseous, 700 bar, from gasification of woody biomass in oxy-fired entrained flow gasifier, with CCS, at fuelling plant</t>
+  </si>
+  <si>
+    <t>Hydrogen, gaseous, 700 bar, from gasification of woody biomass in oxy-fired entrained flow gasifier, at fuelling plant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -352,7 +371,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -360,6 +379,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -639,19 +660,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M187"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" workbookViewId="0">
-      <selection activeCell="I185" sqref="I185"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="A188" sqref="A188"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="41.88671875" customWidth="1"/>
+    <col min="1" max="1" width="60.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>62</v>
       </c>
@@ -659,7 +680,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -667,7 +688,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -675,7 +696,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -683,7 +704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -691,7 +712,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -699,7 +720,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -707,12 +728,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -753,7 +774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>83</v>
       </c>
@@ -782,7 +803,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -820,7 +841,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>80</v>
       </c>
@@ -858,7 +879,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -897,7 +918,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>81</v>
       </c>
@@ -935,7 +956,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>0</v>
       </c>
@@ -943,7 +964,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -951,7 +972,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -959,7 +980,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -967,7 +988,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -975,7 +996,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -983,12 +1004,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -1029,7 +1050,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>84</v>
       </c>
@@ -1058,7 +1079,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -1096,7 +1117,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -1134,7 +1155,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -1173,7 +1194,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1211,7 +1232,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>0</v>
       </c>
@@ -1219,7 +1240,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1248,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1235,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -1243,7 +1264,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>7</v>
       </c>
@@ -1251,7 +1272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1259,12 +1280,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1305,7 +1326,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>85</v>
       </c>
@@ -1334,7 +1355,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -1372,7 +1393,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1410,7 +1431,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>34</v>
       </c>
@@ -1449,7 +1470,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>82</v>
       </c>
@@ -1487,7 +1508,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -1495,7 +1516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -1503,7 +1524,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>4</v>
       </c>
@@ -1511,7 +1532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1519,7 +1540,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>7</v>
       </c>
@@ -1527,7 +1548,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -1535,7 +1556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>11</v>
       </c>
@@ -1543,7 +1564,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -1551,12 +1572,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>16</v>
       </c>
@@ -1579,7 +1600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>1</v>
       </c>
@@ -1602,7 +1623,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>21</v>
       </c>
@@ -1625,7 +1646,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>24</v>
       </c>
@@ -1648,7 +1669,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>29</v>
       </c>
@@ -1668,7 +1689,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>30</v>
       </c>
@@ -1688,7 +1709,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>32</v>
       </c>
@@ -1708,7 +1729,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -1716,7 +1737,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -1724,7 +1745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -1732,7 +1753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>5</v>
       </c>
@@ -1740,7 +1761,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>7</v>
       </c>
@@ -1748,7 +1769,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>9</v>
       </c>
@@ -1756,7 +1777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>11</v>
       </c>
@@ -1764,7 +1785,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>13</v>
       </c>
@@ -1772,12 +1793,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -1800,7 +1821,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>33</v>
       </c>
@@ -1823,7 +1844,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>34</v>
       </c>
@@ -1846,7 +1867,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>24</v>
       </c>
@@ -1869,7 +1890,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>29</v>
       </c>
@@ -1889,7 +1910,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>30</v>
       </c>
@@ -1909,7 +1930,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>32</v>
       </c>
@@ -1929,7 +1950,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>0</v>
       </c>
@@ -1937,7 +1958,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>35</v>
       </c>
@@ -1945,7 +1966,7 @@
         <v>1.6203919960640381</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -1953,7 +1974,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>5</v>
       </c>
@@ -1961,7 +1982,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>9</v>
       </c>
@@ -1969,7 +1990,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>11</v>
       </c>
@@ -1977,7 +1998,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>13</v>
       </c>
@@ -1985,12 +2006,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>16</v>
       </c>
@@ -2016,7 +2037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>34</v>
       </c>
@@ -2039,7 +2060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>38</v>
       </c>
@@ -2065,7 +2086,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>43</v>
       </c>
@@ -2091,7 +2112,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>46</v>
       </c>
@@ -2114,7 +2135,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>47</v>
       </c>
@@ -2137,7 +2158,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>50</v>
       </c>
@@ -2160,7 +2181,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>52</v>
       </c>
@@ -2183,7 +2204,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>55</v>
       </c>
@@ -2206,7 +2227,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>58</v>
       </c>
@@ -2229,7 +2250,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>60</v>
       </c>
@@ -2252,7 +2273,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A99" s="1" t="s">
         <v>0</v>
       </c>
@@ -2260,7 +2281,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>35</v>
       </c>
@@ -2268,7 +2289,7 @@
         <v>1.6203919960640381</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>2</v>
       </c>
@@ -2276,7 +2297,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>5</v>
       </c>
@@ -2284,7 +2305,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>9</v>
       </c>
@@ -2292,7 +2313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>11</v>
       </c>
@@ -2300,7 +2321,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>13</v>
       </c>
@@ -2308,12 +2329,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A106" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>16</v>
       </c>
@@ -2339,7 +2360,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>21</v>
       </c>
@@ -2362,7 +2383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>38</v>
       </c>
@@ -2388,7 +2409,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>43</v>
       </c>
@@ -2414,7 +2435,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>47</v>
       </c>
@@ -2437,7 +2458,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>50</v>
       </c>
@@ -2460,7 +2481,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>52</v>
       </c>
@@ -2483,7 +2504,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>55</v>
       </c>
@@ -2506,7 +2527,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>58</v>
       </c>
@@ -2529,7 +2550,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>60</v>
       </c>
@@ -2552,7 +2573,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A118" s="1" t="s">
         <v>0</v>
       </c>
@@ -2560,7 +2581,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>2</v>
       </c>
@@ -2568,7 +2589,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>4</v>
       </c>
@@ -2576,7 +2597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>5</v>
       </c>
@@ -2584,7 +2605,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>7</v>
       </c>
@@ -2592,7 +2613,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>9</v>
       </c>
@@ -2600,7 +2621,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>11</v>
       </c>
@@ -2608,7 +2629,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>13</v>
       </c>
@@ -2616,12 +2637,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A126" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>16</v>
       </c>
@@ -2644,7 +2665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A128" s="2" t="s">
         <v>74</v>
       </c>
@@ -2667,7 +2688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>75</v>
       </c>
@@ -2690,7 +2711,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>24</v>
       </c>
@@ -2713,7 +2734,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>29</v>
       </c>
@@ -2733,7 +2754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>30</v>
       </c>
@@ -2753,7 +2774,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>32</v>
       </c>
@@ -2773,7 +2794,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A135" s="1" t="s">
         <v>0</v>
       </c>
@@ -2781,7 +2802,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>35</v>
       </c>
@@ -2789,7 +2810,7 @@
         <v>1.4983549435621251</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>2</v>
       </c>
@@ -2797,7 +2818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>5</v>
       </c>
@@ -2805,7 +2826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>9</v>
       </c>
@@ -2813,7 +2834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>11</v>
       </c>
@@ -2821,7 +2842,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>13</v>
       </c>
@@ -2829,12 +2850,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="142" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A142" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>16</v>
       </c>
@@ -2860,7 +2881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="str">
         <f>B135</f>
         <v>Hydrogen, gaseous, 25 bar, from gasification of woody biomass in oxy-fired entrained flow gasifier, with CCS, at gasification plant</v>
@@ -2884,7 +2905,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>38</v>
       </c>
@@ -2910,7 +2931,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>43</v>
       </c>
@@ -2936,7 +2957,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>46</v>
       </c>
@@ -2959,7 +2980,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>47</v>
       </c>
@@ -2982,7 +3003,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>50</v>
       </c>
@@ -3005,7 +3026,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>52</v>
       </c>
@@ -3028,7 +3049,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>55</v>
       </c>
@@ -3051,7 +3072,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>58</v>
       </c>
@@ -3074,7 +3095,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="154" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A154" s="1" t="s">
         <v>0</v>
       </c>
@@ -3082,7 +3103,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>2</v>
       </c>
@@ -3090,7 +3111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>4</v>
       </c>
@@ -3098,7 +3119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>5</v>
       </c>
@@ -3106,7 +3127,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>7</v>
       </c>
@@ -3114,7 +3135,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>9</v>
       </c>
@@ -3122,7 +3143,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>11</v>
       </c>
@@ -3130,7 +3151,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>13</v>
       </c>
@@ -3138,12 +3159,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A162" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>16</v>
       </c>
@@ -3166,7 +3187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
         <v>77</v>
       </c>
@@ -3189,7 +3210,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A165" s="2" t="s">
         <v>78</v>
       </c>
@@ -3212,7 +3233,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>24</v>
       </c>
@@ -3235,7 +3256,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>29</v>
       </c>
@@ -3255,7 +3276,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>30</v>
       </c>
@@ -3275,7 +3296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>32</v>
       </c>
@@ -3295,7 +3316,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A171" s="1" t="s">
         <v>0</v>
       </c>
@@ -3303,7 +3324,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>35</v>
       </c>
@@ -3311,7 +3332,7 @@
         <v>1.4983549435621251</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>2</v>
       </c>
@@ -3319,7 +3340,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>5</v>
       </c>
@@ -3327,7 +3348,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>9</v>
       </c>
@@ -3335,7 +3356,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>11</v>
       </c>
@@ -3343,7 +3364,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>13</v>
       </c>
@@ -3351,12 +3372,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="178" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A178" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>16</v>
       </c>
@@ -3382,7 +3403,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A180" s="2" t="str">
         <f>B171</f>
         <v>Hydrogen, gaseous, 25 bar, from gasification of woody biomass in oxy-fired entrained flow gasifier, at gasification plant</v>
@@ -3406,7 +3427,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>38</v>
       </c>
@@ -3432,7 +3453,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>43</v>
       </c>
@@ -3458,7 +3479,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>47</v>
       </c>
@@ -3481,7 +3502,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>50</v>
       </c>
@@ -3504,7 +3525,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>52</v>
       </c>
@@ -3527,7 +3548,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>55</v>
       </c>
@@ -3550,7 +3571,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>58</v>
       </c>
@@ -3570,6 +3591,2092 @@
         <v>22</v>
       </c>
       <c r="H187" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>2</v>
+      </c>
+      <c r="B190" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>4</v>
+      </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>5</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>7</v>
+      </c>
+      <c r="B193" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>9</v>
+      </c>
+      <c r="B194" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A195" t="s">
+        <v>11</v>
+      </c>
+      <c r="B195" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A196" t="s">
+        <v>13</v>
+      </c>
+      <c r="B196" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A197" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A198" t="s">
+        <v>16</v>
+      </c>
+      <c r="B198" t="s">
+        <v>17</v>
+      </c>
+      <c r="C198" t="s">
+        <v>18</v>
+      </c>
+      <c r="D198" t="s">
+        <v>2</v>
+      </c>
+      <c r="E198" t="s">
+        <v>9</v>
+      </c>
+      <c r="F198" t="s">
+        <v>7</v>
+      </c>
+      <c r="G198" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A199" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B199">
+        <v>1</v>
+      </c>
+      <c r="C199" t="s">
+        <v>19</v>
+      </c>
+      <c r="D199" t="s">
+        <v>26</v>
+      </c>
+      <c r="E199" t="s">
+        <v>10</v>
+      </c>
+      <c r="F199" t="s">
+        <v>20</v>
+      </c>
+      <c r="G199" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A200" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B200">
+        <v>1</v>
+      </c>
+      <c r="C200" t="s">
+        <v>19</v>
+      </c>
+      <c r="D200" t="s">
+        <v>26</v>
+      </c>
+      <c r="E200" t="s">
+        <v>10</v>
+      </c>
+      <c r="F200" t="s">
+        <v>22</v>
+      </c>
+      <c r="G200" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A201" t="s">
+        <v>24</v>
+      </c>
+      <c r="B201">
+        <v>3.2</v>
+      </c>
+      <c r="C201" t="s">
+        <v>25</v>
+      </c>
+      <c r="D201" t="s">
+        <v>26</v>
+      </c>
+      <c r="E201" t="s">
+        <v>27</v>
+      </c>
+      <c r="F201" t="s">
+        <v>22</v>
+      </c>
+      <c r="G201" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A202" t="s">
+        <v>29</v>
+      </c>
+      <c r="B202">
+        <v>1.6931E-7</v>
+      </c>
+      <c r="C202" t="s">
+        <v>19</v>
+      </c>
+      <c r="D202" t="s">
+        <v>26</v>
+      </c>
+      <c r="E202" t="s">
+        <v>9</v>
+      </c>
+      <c r="F202" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A203" t="s">
+        <v>30</v>
+      </c>
+      <c r="B203">
+        <v>1.6931E-7</v>
+      </c>
+      <c r="C203" t="s">
+        <v>19</v>
+      </c>
+      <c r="D203" t="s">
+        <v>31</v>
+      </c>
+      <c r="E203" t="s">
+        <v>9</v>
+      </c>
+      <c r="F203" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A204" t="s">
+        <v>32</v>
+      </c>
+      <c r="B204">
+        <v>1.6930571108622621E-7</v>
+      </c>
+      <c r="C204" t="s">
+        <v>19</v>
+      </c>
+      <c r="D204" t="s">
+        <v>31</v>
+      </c>
+      <c r="E204" t="s">
+        <v>9</v>
+      </c>
+      <c r="F204" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="206" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A206" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A207" t="s">
+        <v>2</v>
+      </c>
+      <c r="B207" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A208" t="s">
+        <v>4</v>
+      </c>
+      <c r="B208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A209" t="s">
+        <v>5</v>
+      </c>
+      <c r="B209" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A210" t="s">
+        <v>7</v>
+      </c>
+      <c r="B210" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A211" t="s">
+        <v>9</v>
+      </c>
+      <c r="B211" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A212" t="s">
+        <v>11</v>
+      </c>
+      <c r="B212" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A213" t="s">
+        <v>13</v>
+      </c>
+      <c r="B213" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A214" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A215" t="s">
+        <v>16</v>
+      </c>
+      <c r="B215" t="s">
+        <v>17</v>
+      </c>
+      <c r="C215" t="s">
+        <v>18</v>
+      </c>
+      <c r="D215" t="s">
+        <v>2</v>
+      </c>
+      <c r="E215" t="s">
+        <v>9</v>
+      </c>
+      <c r="F215" t="s">
+        <v>7</v>
+      </c>
+      <c r="G215" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="216" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A216" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B216">
+        <v>1</v>
+      </c>
+      <c r="C216" t="s">
+        <v>19</v>
+      </c>
+      <c r="D216" t="s">
+        <v>26</v>
+      </c>
+      <c r="E216" t="s">
+        <v>10</v>
+      </c>
+      <c r="F216" t="s">
+        <v>20</v>
+      </c>
+      <c r="G216" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="217" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A217" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B217">
+        <v>1</v>
+      </c>
+      <c r="C217" t="s">
+        <v>19</v>
+      </c>
+      <c r="D217" t="s">
+        <v>26</v>
+      </c>
+      <c r="E217" t="s">
+        <v>10</v>
+      </c>
+      <c r="F217" t="s">
+        <v>22</v>
+      </c>
+      <c r="G217" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A218" t="s">
+        <v>24</v>
+      </c>
+      <c r="B218">
+        <v>3.2</v>
+      </c>
+      <c r="C218" t="s">
+        <v>25</v>
+      </c>
+      <c r="D218" t="s">
+        <v>26</v>
+      </c>
+      <c r="E218" t="s">
+        <v>27</v>
+      </c>
+      <c r="F218" t="s">
+        <v>22</v>
+      </c>
+      <c r="G218" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A219" t="s">
+        <v>29</v>
+      </c>
+      <c r="B219">
+        <v>1.6931E-7</v>
+      </c>
+      <c r="C219" t="s">
+        <v>19</v>
+      </c>
+      <c r="D219" t="s">
+        <v>26</v>
+      </c>
+      <c r="E219" t="s">
+        <v>9</v>
+      </c>
+      <c r="F219" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A220" t="s">
+        <v>30</v>
+      </c>
+      <c r="B220">
+        <v>1.6931E-7</v>
+      </c>
+      <c r="C220" t="s">
+        <v>19</v>
+      </c>
+      <c r="D220" t="s">
+        <v>31</v>
+      </c>
+      <c r="E220" t="s">
+        <v>9</v>
+      </c>
+      <c r="F220" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A221" t="s">
+        <v>32</v>
+      </c>
+      <c r="B221">
+        <v>1.6930571108622621E-7</v>
+      </c>
+      <c r="C221" t="s">
+        <v>19</v>
+      </c>
+      <c r="D221" t="s">
+        <v>31</v>
+      </c>
+      <c r="E221" t="s">
+        <v>9</v>
+      </c>
+      <c r="F221" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="223" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A223" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A224" t="s">
+        <v>35</v>
+      </c>
+      <c r="B224" s="7">
+        <v>1.8132045976445506</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A225" t="s">
+        <v>2</v>
+      </c>
+      <c r="B225" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>5</v>
+      </c>
+      <c r="B226" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A227" t="s">
+        <v>9</v>
+      </c>
+      <c r="B227" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A228" t="s">
+        <v>11</v>
+      </c>
+      <c r="B228" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A229" t="s">
+        <v>13</v>
+      </c>
+      <c r="B229" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A230" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A231" t="s">
+        <v>16</v>
+      </c>
+      <c r="B231" t="s">
+        <v>17</v>
+      </c>
+      <c r="C231" t="s">
+        <v>18</v>
+      </c>
+      <c r="D231" t="s">
+        <v>2</v>
+      </c>
+      <c r="E231" t="s">
+        <v>9</v>
+      </c>
+      <c r="F231" t="s">
+        <v>37</v>
+      </c>
+      <c r="G231" t="s">
+        <v>7</v>
+      </c>
+      <c r="H231" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A232" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B232">
+        <v>1</v>
+      </c>
+      <c r="C232" t="s">
+        <v>19</v>
+      </c>
+      <c r="D232" t="s">
+        <v>26</v>
+      </c>
+      <c r="E232" t="s">
+        <v>10</v>
+      </c>
+      <c r="G232" t="s">
+        <v>20</v>
+      </c>
+      <c r="H232" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A233" t="s">
+        <v>38</v>
+      </c>
+      <c r="B233">
+        <v>8.3668780583516718</v>
+      </c>
+      <c r="C233" t="s">
+        <v>39</v>
+      </c>
+      <c r="D233" t="s">
+        <v>40</v>
+      </c>
+      <c r="E233" t="s">
+        <v>10</v>
+      </c>
+      <c r="F233" t="s">
+        <v>41</v>
+      </c>
+      <c r="G233" t="s">
+        <v>42</v>
+      </c>
+      <c r="H233" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A234" t="s">
+        <v>43</v>
+      </c>
+      <c r="B234" s="6">
+        <v>0.38041197561668283</v>
+      </c>
+      <c r="C234" t="s">
+        <v>39</v>
+      </c>
+      <c r="D234" t="s">
+        <v>40</v>
+      </c>
+      <c r="E234" t="s">
+        <v>44</v>
+      </c>
+      <c r="F234" t="s">
+        <v>45</v>
+      </c>
+      <c r="G234" t="s">
+        <v>42</v>
+      </c>
+      <c r="H234" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A235" t="s">
+        <v>46</v>
+      </c>
+      <c r="B235">
+        <v>12.493810765991332</v>
+      </c>
+      <c r="C235" t="s">
+        <v>19</v>
+      </c>
+      <c r="D235" t="s">
+        <v>26</v>
+      </c>
+      <c r="E235" t="s">
+        <v>10</v>
+      </c>
+      <c r="G235" t="s">
+        <v>22</v>
+      </c>
+      <c r="H235" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A236" t="s">
+        <v>47</v>
+      </c>
+      <c r="B236">
+        <v>2.54628E-9</v>
+      </c>
+      <c r="C236" t="s">
+        <v>48</v>
+      </c>
+      <c r="D236" t="s">
+        <v>31</v>
+      </c>
+      <c r="E236" t="s">
+        <v>9</v>
+      </c>
+      <c r="G236" t="s">
+        <v>22</v>
+      </c>
+      <c r="H236" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A237" t="s">
+        <v>50</v>
+      </c>
+      <c r="B237">
+        <v>7.5390157563601576</v>
+      </c>
+      <c r="C237" t="s">
+        <v>48</v>
+      </c>
+      <c r="D237" t="s">
+        <v>88</v>
+      </c>
+      <c r="E237" t="s">
+        <v>10</v>
+      </c>
+      <c r="G237" t="s">
+        <v>22</v>
+      </c>
+      <c r="H237" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A238" t="s">
+        <v>52</v>
+      </c>
+      <c r="B238">
+        <v>11.512410143774924</v>
+      </c>
+      <c r="C238" t="s">
+        <v>53</v>
+      </c>
+      <c r="D238" t="s">
+        <v>88</v>
+      </c>
+      <c r="E238" t="s">
+        <v>10</v>
+      </c>
+      <c r="G238" t="s">
+        <v>22</v>
+      </c>
+      <c r="H238" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A239" t="s">
+        <v>55</v>
+      </c>
+      <c r="B239">
+        <v>3.8560069111530564</v>
+      </c>
+      <c r="C239" t="s">
+        <v>48</v>
+      </c>
+      <c r="D239" t="s">
+        <v>56</v>
+      </c>
+      <c r="E239" t="s">
+        <v>27</v>
+      </c>
+      <c r="G239" t="s">
+        <v>22</v>
+      </c>
+      <c r="H239" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A240" t="s">
+        <v>58</v>
+      </c>
+      <c r="B240">
+        <v>5.3483199147628007E-10</v>
+      </c>
+      <c r="C240" t="s">
+        <v>48</v>
+      </c>
+      <c r="D240" t="s">
+        <v>3</v>
+      </c>
+      <c r="E240" t="s">
+        <v>9</v>
+      </c>
+      <c r="G240" t="s">
+        <v>22</v>
+      </c>
+      <c r="H240" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A241" t="s">
+        <v>60</v>
+      </c>
+      <c r="B241">
+        <v>2.8615461179087874E-7</v>
+      </c>
+      <c r="C241" t="s">
+        <v>48</v>
+      </c>
+      <c r="D241" t="s">
+        <v>3</v>
+      </c>
+      <c r="E241" t="s">
+        <v>10</v>
+      </c>
+      <c r="G241" t="s">
+        <v>22</v>
+      </c>
+      <c r="H241" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A243" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A244" t="s">
+        <v>35</v>
+      </c>
+      <c r="B244">
+        <v>1.8132045976445506</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A245" t="s">
+        <v>2</v>
+      </c>
+      <c r="B245" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A246" t="s">
+        <v>5</v>
+      </c>
+      <c r="B246" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A247" t="s">
+        <v>9</v>
+      </c>
+      <c r="B247" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A248" t="s">
+        <v>11</v>
+      </c>
+      <c r="B248" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A249" t="s">
+        <v>13</v>
+      </c>
+      <c r="B249" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A250" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A251" t="s">
+        <v>16</v>
+      </c>
+      <c r="B251" t="s">
+        <v>17</v>
+      </c>
+      <c r="C251" t="s">
+        <v>18</v>
+      </c>
+      <c r="D251" t="s">
+        <v>2</v>
+      </c>
+      <c r="E251" t="s">
+        <v>9</v>
+      </c>
+      <c r="F251" t="s">
+        <v>37</v>
+      </c>
+      <c r="G251" t="s">
+        <v>7</v>
+      </c>
+      <c r="H251" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A252" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B252">
+        <v>1</v>
+      </c>
+      <c r="C252" t="s">
+        <v>19</v>
+      </c>
+      <c r="D252" t="s">
+        <v>26</v>
+      </c>
+      <c r="E252" t="s">
+        <v>10</v>
+      </c>
+      <c r="G252" t="s">
+        <v>20</v>
+      </c>
+      <c r="H252" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A253" t="s">
+        <v>38</v>
+      </c>
+      <c r="B253">
+        <v>20.860692830127658</v>
+      </c>
+      <c r="C253" t="s">
+        <v>39</v>
+      </c>
+      <c r="D253" t="s">
+        <v>40</v>
+      </c>
+      <c r="E253" t="s">
+        <v>10</v>
+      </c>
+      <c r="F253" t="s">
+        <v>41</v>
+      </c>
+      <c r="G253" t="s">
+        <v>42</v>
+      </c>
+      <c r="H253" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A254" t="s">
+        <v>43</v>
+      </c>
+      <c r="B254">
+        <v>0.38041197561668283</v>
+      </c>
+      <c r="C254" t="s">
+        <v>39</v>
+      </c>
+      <c r="D254" t="s">
+        <v>40</v>
+      </c>
+      <c r="E254" t="s">
+        <v>44</v>
+      </c>
+      <c r="F254" t="s">
+        <v>45</v>
+      </c>
+      <c r="G254" t="s">
+        <v>42</v>
+      </c>
+      <c r="H254" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A255" t="s">
+        <v>47</v>
+      </c>
+      <c r="B255">
+        <v>2.54628E-9</v>
+      </c>
+      <c r="C255" t="s">
+        <v>48</v>
+      </c>
+      <c r="D255" t="s">
+        <v>31</v>
+      </c>
+      <c r="E255" t="s">
+        <v>9</v>
+      </c>
+      <c r="G255" t="s">
+        <v>22</v>
+      </c>
+      <c r="H255" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A256" t="s">
+        <v>50</v>
+      </c>
+      <c r="B256">
+        <v>7.5390157563601576</v>
+      </c>
+      <c r="C256" t="s">
+        <v>48</v>
+      </c>
+      <c r="D256" t="s">
+        <v>88</v>
+      </c>
+      <c r="E256" t="s">
+        <v>10</v>
+      </c>
+      <c r="G256" t="s">
+        <v>22</v>
+      </c>
+      <c r="H256" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A257" t="s">
+        <v>52</v>
+      </c>
+      <c r="B257">
+        <v>11.512410143774924</v>
+      </c>
+      <c r="C257" t="s">
+        <v>53</v>
+      </c>
+      <c r="D257" t="s">
+        <v>88</v>
+      </c>
+      <c r="E257" t="s">
+        <v>10</v>
+      </c>
+      <c r="G257" t="s">
+        <v>22</v>
+      </c>
+      <c r="H257" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A258" t="s">
+        <v>55</v>
+      </c>
+      <c r="B258">
+        <v>1.6298450280608925</v>
+      </c>
+      <c r="C258" t="s">
+        <v>48</v>
+      </c>
+      <c r="D258" t="s">
+        <v>56</v>
+      </c>
+      <c r="E258" t="s">
+        <v>27</v>
+      </c>
+      <c r="G258" t="s">
+        <v>22</v>
+      </c>
+      <c r="H258" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="259" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A259" t="s">
+        <v>58</v>
+      </c>
+      <c r="B259">
+        <v>5.3483199147628007E-10</v>
+      </c>
+      <c r="C259" t="s">
+        <v>48</v>
+      </c>
+      <c r="D259" t="s">
+        <v>3</v>
+      </c>
+      <c r="E259" t="s">
+        <v>9</v>
+      </c>
+      <c r="G259" t="s">
+        <v>22</v>
+      </c>
+      <c r="H259" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A260" t="s">
+        <v>60</v>
+      </c>
+      <c r="B260">
+        <v>2.8615461179087874E-7</v>
+      </c>
+      <c r="C260" t="s">
+        <v>48</v>
+      </c>
+      <c r="D260" t="s">
+        <v>3</v>
+      </c>
+      <c r="E260" t="s">
+        <v>10</v>
+      </c>
+      <c r="G260" t="s">
+        <v>22</v>
+      </c>
+      <c r="H260" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="262" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A262" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B262" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="263" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A263" t="s">
+        <v>2</v>
+      </c>
+      <c r="B263" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="264" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A264" t="s">
+        <v>4</v>
+      </c>
+      <c r="B264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A265" t="s">
+        <v>5</v>
+      </c>
+      <c r="B265" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="266" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A266" t="s">
+        <v>7</v>
+      </c>
+      <c r="B266" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A267" t="s">
+        <v>9</v>
+      </c>
+      <c r="B267" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A268" t="s">
+        <v>11</v>
+      </c>
+      <c r="B268" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A269" t="s">
+        <v>13</v>
+      </c>
+      <c r="B269" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A270" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A271" t="s">
+        <v>16</v>
+      </c>
+      <c r="B271" t="s">
+        <v>17</v>
+      </c>
+      <c r="C271" t="s">
+        <v>18</v>
+      </c>
+      <c r="D271" t="s">
+        <v>2</v>
+      </c>
+      <c r="E271" t="s">
+        <v>9</v>
+      </c>
+      <c r="F271" t="s">
+        <v>7</v>
+      </c>
+      <c r="G271" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A272" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B272">
+        <v>1</v>
+      </c>
+      <c r="C272" t="s">
+        <v>19</v>
+      </c>
+      <c r="D272" t="s">
+        <v>26</v>
+      </c>
+      <c r="E272" t="s">
+        <v>10</v>
+      </c>
+      <c r="F272" t="s">
+        <v>20</v>
+      </c>
+      <c r="G272" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="273" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A273" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B273">
+        <v>1</v>
+      </c>
+      <c r="C273" t="s">
+        <v>19</v>
+      </c>
+      <c r="D273" t="s">
+        <v>26</v>
+      </c>
+      <c r="E273" t="s">
+        <v>10</v>
+      </c>
+      <c r="F273" t="s">
+        <v>22</v>
+      </c>
+      <c r="G273" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A274" t="s">
+        <v>24</v>
+      </c>
+      <c r="B274">
+        <v>3.2</v>
+      </c>
+      <c r="C274" t="s">
+        <v>25</v>
+      </c>
+      <c r="D274" t="s">
+        <v>26</v>
+      </c>
+      <c r="E274" t="s">
+        <v>27</v>
+      </c>
+      <c r="F274" t="s">
+        <v>22</v>
+      </c>
+      <c r="G274" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A275" t="s">
+        <v>29</v>
+      </c>
+      <c r="B275">
+        <v>1.6931E-7</v>
+      </c>
+      <c r="C275" t="s">
+        <v>19</v>
+      </c>
+      <c r="D275" t="s">
+        <v>26</v>
+      </c>
+      <c r="E275" t="s">
+        <v>9</v>
+      </c>
+      <c r="F275" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="276" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A276" t="s">
+        <v>30</v>
+      </c>
+      <c r="B276">
+        <v>1.6931E-7</v>
+      </c>
+      <c r="C276" t="s">
+        <v>19</v>
+      </c>
+      <c r="D276" t="s">
+        <v>31</v>
+      </c>
+      <c r="E276" t="s">
+        <v>9</v>
+      </c>
+      <c r="F276" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A277" t="s">
+        <v>32</v>
+      </c>
+      <c r="B277">
+        <v>1.6930571108622621E-7</v>
+      </c>
+      <c r="C277" t="s">
+        <v>19</v>
+      </c>
+      <c r="D277" t="s">
+        <v>31</v>
+      </c>
+      <c r="E277" t="s">
+        <v>9</v>
+      </c>
+      <c r="F277" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="279" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A279" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="280" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A280" t="s">
+        <v>35</v>
+      </c>
+      <c r="B280" s="8">
+        <v>1.4983549435621251</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A281" t="s">
+        <v>2</v>
+      </c>
+      <c r="B281" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A282" t="s">
+        <v>5</v>
+      </c>
+      <c r="B282" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A283" t="s">
+        <v>9</v>
+      </c>
+      <c r="B283" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A284" t="s">
+        <v>11</v>
+      </c>
+      <c r="B284" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A285" t="s">
+        <v>13</v>
+      </c>
+      <c r="B285" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A286" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A287" t="s">
+        <v>16</v>
+      </c>
+      <c r="B287" t="s">
+        <v>17</v>
+      </c>
+      <c r="C287" t="s">
+        <v>18</v>
+      </c>
+      <c r="D287" t="s">
+        <v>2</v>
+      </c>
+      <c r="E287" t="s">
+        <v>9</v>
+      </c>
+      <c r="F287" t="s">
+        <v>37</v>
+      </c>
+      <c r="G287" t="s">
+        <v>7</v>
+      </c>
+      <c r="H287" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="288" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A288" s="2" t="str">
+        <f>B279</f>
+        <v>Hydrogen, gaseous, 25 bar, from gasification of woody biomass in oxy-fired entrained flow gasifier, with CCS, at gasification plant</v>
+      </c>
+      <c r="B288">
+        <v>1</v>
+      </c>
+      <c r="C288" t="s">
+        <v>19</v>
+      </c>
+      <c r="D288" t="s">
+        <v>26</v>
+      </c>
+      <c r="E288" t="s">
+        <v>10</v>
+      </c>
+      <c r="G288" t="s">
+        <v>20</v>
+      </c>
+      <c r="H288" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A289" t="s">
+        <v>38</v>
+      </c>
+      <c r="B289">
+        <v>0.43169673539678227</v>
+      </c>
+      <c r="C289" t="s">
+        <v>39</v>
+      </c>
+      <c r="D289" t="s">
+        <v>40</v>
+      </c>
+      <c r="E289" t="s">
+        <v>10</v>
+      </c>
+      <c r="F289" t="s">
+        <v>41</v>
+      </c>
+      <c r="G289" t="s">
+        <v>42</v>
+      </c>
+      <c r="H289" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A290" t="s">
+        <v>43</v>
+      </c>
+      <c r="B290" s="6">
+        <v>0.38041197561668283</v>
+      </c>
+      <c r="C290" t="s">
+        <v>39</v>
+      </c>
+      <c r="D290" t="s">
+        <v>40</v>
+      </c>
+      <c r="E290" t="s">
+        <v>44</v>
+      </c>
+      <c r="F290" t="s">
+        <v>45</v>
+      </c>
+      <c r="G290" t="s">
+        <v>42</v>
+      </c>
+      <c r="H290" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A291" t="s">
+        <v>46</v>
+      </c>
+      <c r="B291">
+        <v>16.76304418862647</v>
+      </c>
+      <c r="C291" t="s">
+        <v>19</v>
+      </c>
+      <c r="D291" t="s">
+        <v>26</v>
+      </c>
+      <c r="E291" t="s">
+        <v>10</v>
+      </c>
+      <c r="G291" t="s">
+        <v>22</v>
+      </c>
+      <c r="H291" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A292" t="s">
+        <v>47</v>
+      </c>
+      <c r="B292">
+        <v>2.54628E-9</v>
+      </c>
+      <c r="C292" t="s">
+        <v>48</v>
+      </c>
+      <c r="D292" t="s">
+        <v>31</v>
+      </c>
+      <c r="E292" t="s">
+        <v>9</v>
+      </c>
+      <c r="G292" t="s">
+        <v>22</v>
+      </c>
+      <c r="H292" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A293" t="s">
+        <v>50</v>
+      </c>
+      <c r="B293">
+        <v>7.5390157563601576</v>
+      </c>
+      <c r="C293" t="s">
+        <v>48</v>
+      </c>
+      <c r="D293" t="s">
+        <v>88</v>
+      </c>
+      <c r="E293" t="s">
+        <v>10</v>
+      </c>
+      <c r="G293" t="s">
+        <v>22</v>
+      </c>
+      <c r="H293" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A294" t="s">
+        <v>52</v>
+      </c>
+      <c r="B294">
+        <v>9.5133647210293653</v>
+      </c>
+      <c r="C294" t="s">
+        <v>53</v>
+      </c>
+      <c r="D294" t="s">
+        <v>88</v>
+      </c>
+      <c r="E294" t="s">
+        <v>10</v>
+      </c>
+      <c r="G294" t="s">
+        <v>22</v>
+      </c>
+      <c r="H294" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A295" t="s">
+        <v>55</v>
+      </c>
+      <c r="B295">
+        <v>0.20061042458473774</v>
+      </c>
+      <c r="C295" t="s">
+        <v>48</v>
+      </c>
+      <c r="D295" t="s">
+        <v>56</v>
+      </c>
+      <c r="E295" t="s">
+        <v>27</v>
+      </c>
+      <c r="G295" t="s">
+        <v>22</v>
+      </c>
+      <c r="H295" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="296" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A296" t="s">
+        <v>58</v>
+      </c>
+      <c r="B296">
+        <v>5.3483199147628007E-10</v>
+      </c>
+      <c r="C296" t="s">
+        <v>48</v>
+      </c>
+      <c r="D296" t="s">
+        <v>3</v>
+      </c>
+      <c r="E296" t="s">
+        <v>9</v>
+      </c>
+      <c r="G296" t="s">
+        <v>22</v>
+      </c>
+      <c r="H296" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A298" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B298" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A299" t="s">
+        <v>2</v>
+      </c>
+      <c r="B299" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A300" t="s">
+        <v>4</v>
+      </c>
+      <c r="B300">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A301" t="s">
+        <v>5</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A302" t="s">
+        <v>7</v>
+      </c>
+      <c r="B302" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A303" t="s">
+        <v>9</v>
+      </c>
+      <c r="B303" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A304" t="s">
+        <v>11</v>
+      </c>
+      <c r="B304" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A305" t="s">
+        <v>13</v>
+      </c>
+      <c r="B305" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A306" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A307" t="s">
+        <v>16</v>
+      </c>
+      <c r="B307" t="s">
+        <v>17</v>
+      </c>
+      <c r="C307" t="s">
+        <v>18</v>
+      </c>
+      <c r="D307" t="s">
+        <v>2</v>
+      </c>
+      <c r="E307" t="s">
+        <v>9</v>
+      </c>
+      <c r="F307" t="s">
+        <v>7</v>
+      </c>
+      <c r="G307" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A308" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B308">
+        <v>1</v>
+      </c>
+      <c r="C308" t="s">
+        <v>19</v>
+      </c>
+      <c r="D308" t="s">
+        <v>26</v>
+      </c>
+      <c r="E308" t="s">
+        <v>10</v>
+      </c>
+      <c r="F308" t="s">
+        <v>20</v>
+      </c>
+      <c r="G308" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A309" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B309">
+        <v>1</v>
+      </c>
+      <c r="C309" t="s">
+        <v>19</v>
+      </c>
+      <c r="D309" t="s">
+        <v>26</v>
+      </c>
+      <c r="E309" t="s">
+        <v>10</v>
+      </c>
+      <c r="F309" t="s">
+        <v>22</v>
+      </c>
+      <c r="G309" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A310" t="s">
+        <v>24</v>
+      </c>
+      <c r="B310">
+        <v>3.2</v>
+      </c>
+      <c r="C310" t="s">
+        <v>25</v>
+      </c>
+      <c r="D310" t="s">
+        <v>26</v>
+      </c>
+      <c r="E310" t="s">
+        <v>27</v>
+      </c>
+      <c r="F310" t="s">
+        <v>22</v>
+      </c>
+      <c r="G310" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A311" t="s">
+        <v>29</v>
+      </c>
+      <c r="B311">
+        <v>1.6931E-7</v>
+      </c>
+      <c r="C311" t="s">
+        <v>19</v>
+      </c>
+      <c r="D311" t="s">
+        <v>26</v>
+      </c>
+      <c r="E311" t="s">
+        <v>9</v>
+      </c>
+      <c r="F311" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
+        <v>30</v>
+      </c>
+      <c r="B312">
+        <v>1.6931E-7</v>
+      </c>
+      <c r="C312" t="s">
+        <v>19</v>
+      </c>
+      <c r="D312" t="s">
+        <v>31</v>
+      </c>
+      <c r="E312" t="s">
+        <v>9</v>
+      </c>
+      <c r="F312" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
+        <v>32</v>
+      </c>
+      <c r="B313">
+        <v>1.6930571108622621E-7</v>
+      </c>
+      <c r="C313" t="s">
+        <v>19</v>
+      </c>
+      <c r="D313" t="s">
+        <v>31</v>
+      </c>
+      <c r="E313" t="s">
+        <v>9</v>
+      </c>
+      <c r="F313" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A315" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
+        <v>35</v>
+      </c>
+      <c r="B316">
+        <v>1.4983549435621251</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>2</v>
+      </c>
+      <c r="B317" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
+        <v>5</v>
+      </c>
+      <c r="B318" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
+        <v>9</v>
+      </c>
+      <c r="B319" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A320" t="s">
+        <v>11</v>
+      </c>
+      <c r="B320" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="321" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
+        <v>13</v>
+      </c>
+      <c r="B321" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="322" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A322" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="323" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A323" t="s">
+        <v>16</v>
+      </c>
+      <c r="B323" t="s">
+        <v>17</v>
+      </c>
+      <c r="C323" t="s">
+        <v>18</v>
+      </c>
+      <c r="D323" t="s">
+        <v>2</v>
+      </c>
+      <c r="E323" t="s">
+        <v>9</v>
+      </c>
+      <c r="F323" t="s">
+        <v>37</v>
+      </c>
+      <c r="G323" t="s">
+        <v>7</v>
+      </c>
+      <c r="H323" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="324" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A324" s="2" t="str">
+        <f>B315</f>
+        <v>Hydrogen, gaseous, 25 bar, from gasification of woody biomass in oxy-fired entrained flow gasifier, at gasification plant</v>
+      </c>
+      <c r="B324">
+        <v>1</v>
+      </c>
+      <c r="C324" t="s">
+        <v>19</v>
+      </c>
+      <c r="D324" t="s">
+        <v>26</v>
+      </c>
+      <c r="E324" t="s">
+        <v>10</v>
+      </c>
+      <c r="G324" t="s">
+        <v>20</v>
+      </c>
+      <c r="H324" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="325" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A325" t="s">
+        <v>38</v>
+      </c>
+      <c r="B325">
+        <v>17.194741369110432</v>
+      </c>
+      <c r="C325" t="s">
+        <v>39</v>
+      </c>
+      <c r="D325" t="s">
+        <v>40</v>
+      </c>
+      <c r="E325" t="s">
+        <v>10</v>
+      </c>
+      <c r="F325" t="s">
+        <v>41</v>
+      </c>
+      <c r="G325" t="s">
+        <v>42</v>
+      </c>
+      <c r="H325" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="326" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A326" t="s">
+        <v>43</v>
+      </c>
+      <c r="B326">
+        <v>0.38041197561668283</v>
+      </c>
+      <c r="C326" t="s">
+        <v>39</v>
+      </c>
+      <c r="D326" t="s">
+        <v>40</v>
+      </c>
+      <c r="E326" t="s">
+        <v>44</v>
+      </c>
+      <c r="F326" t="s">
+        <v>45</v>
+      </c>
+      <c r="G326" t="s">
+        <v>42</v>
+      </c>
+      <c r="H326" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="327" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A327" t="s">
+        <v>47</v>
+      </c>
+      <c r="B327">
+        <v>2.54628E-9</v>
+      </c>
+      <c r="C327" t="s">
+        <v>48</v>
+      </c>
+      <c r="D327" t="s">
+        <v>31</v>
+      </c>
+      <c r="E327" t="s">
+        <v>9</v>
+      </c>
+      <c r="G327" t="s">
+        <v>22</v>
+      </c>
+      <c r="H327" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="328" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A328" t="s">
+        <v>50</v>
+      </c>
+      <c r="B328">
+        <v>7.5390157563601576</v>
+      </c>
+      <c r="C328" t="s">
+        <v>48</v>
+      </c>
+      <c r="D328" t="s">
+        <v>88</v>
+      </c>
+      <c r="E328" t="s">
+        <v>10</v>
+      </c>
+      <c r="G328" t="s">
+        <v>22</v>
+      </c>
+      <c r="H328" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="329" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A329" t="s">
+        <v>52</v>
+      </c>
+      <c r="B329">
+        <v>9.5133647210293653</v>
+      </c>
+      <c r="C329" t="s">
+        <v>53</v>
+      </c>
+      <c r="D329" t="s">
+        <v>88</v>
+      </c>
+      <c r="E329" t="s">
+        <v>10</v>
+      </c>
+      <c r="G329" t="s">
+        <v>22</v>
+      </c>
+      <c r="H329" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="330" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A330" t="s">
+        <v>55</v>
+      </c>
+      <c r="B330">
+        <v>-2.9711377863811488</v>
+      </c>
+      <c r="C330" t="s">
+        <v>48</v>
+      </c>
+      <c r="D330" t="s">
+        <v>56</v>
+      </c>
+      <c r="E330" t="s">
+        <v>27</v>
+      </c>
+      <c r="G330" t="s">
+        <v>22</v>
+      </c>
+      <c r="H330" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="331" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A331" t="s">
+        <v>58</v>
+      </c>
+      <c r="B331">
+        <v>5.3483199147628007E-10</v>
+      </c>
+      <c r="C331" t="s">
+        <v>48</v>
+      </c>
+      <c r="D331" t="s">
+        <v>3</v>
+      </c>
+      <c r="E331" t="s">
+        <v>9</v>
+      </c>
+      <c r="G331" t="s">
+        <v>22</v>
+      </c>
+      <c r="H331" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>